<commit_message>
display workflow in main, small adjustments in docstrings and README
</commit_message>
<xml_diff>
--- a/results/confront_files/metaphor_confront.xlsx
+++ b/results/confront_files/metaphor_confront.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrac\Documents\Uni\Embeddings\metaphor_experiment\results\confront_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{46416F19-8F78-439A-A26F-5D99391D3A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7570F483-66CE-4A0E-AFD7-1D70630CB014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metaphor_confront" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,7 +696,7 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="44">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -722,46 +722,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
@@ -786,46 +746,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
@@ -850,616 +770,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
@@ -1554,6 +864,296 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1579,28 +1179,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:P11" totalsRowShown="0">
-  <autoFilter ref="A1:P11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:P11" totalsRowShown="0">
+  <autoFilter ref="A1:P11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P11">
     <sortCondition ref="A1:A11"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="metaphor"/>
-    <tableColumn id="2" name="mean_similarity"/>
-    <tableColumn id="3" name="mean_baseline_savedBL" dataDxfId="82"/>
-    <tableColumn id="4" name="mean_baseline_mixedBL" dataDxfId="81"/>
-    <tableColumn id="5" name="mean_test_stat_savedBL" dataDxfId="80"/>
-    <tableColumn id="6" name="mean_test_stat_mixedBL" dataDxfId="79"/>
-    <tableColumn id="7" name="mean_p_value_savedBL" dataDxfId="13"/>
-    <tableColumn id="8" name="mean_p_value_mixedBL" dataDxfId="12"/>
-    <tableColumn id="9" name="amount_pos_sign_savedBL" dataDxfId="78"/>
-    <tableColumn id="10" name="amount_pos_sign_mixedBL" dataDxfId="77"/>
-    <tableColumn id="11" name="amount_pos_insign_savedBL" dataDxfId="76"/>
-    <tableColumn id="12" name="amount_pos_insign_mixedBL" dataDxfId="75"/>
-    <tableColumn id="13" name="amount_neg_sign_savedBL" dataDxfId="7"/>
-    <tableColumn id="14" name="amount_neg_sign_mixedBL" dataDxfId="6"/>
-    <tableColumn id="15" name="amount_neg_insign_savedBL" dataDxfId="1"/>
-    <tableColumn id="16" name="amount_neg_insign_mixedBL" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="metaphor"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="mean_similarity"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="mean_baseline_savedBL" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="mean_baseline_mixedBL" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="mean_test_stat_savedBL" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="mean_test_stat_mixedBL" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="mean_p_value_savedBL" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="mean_p_value_mixedBL" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="amount_pos_sign_savedBL" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="amount_pos_sign_mixedBL" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="amount_pos_insign_savedBL" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="amount_pos_insign_mixedBL" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="amount_neg_sign_savedBL" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="amount_neg_sign_mixedBL" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="amount_neg_insign_savedBL" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="amount_neg_insign_mixedBL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1902,7 +1502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2480,64 +2080,64 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="top10" dxfId="54" priority="30" percent="1" rank="10"/>
-    <cfRule type="top10" dxfId="53" priority="29" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="29" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="top10" dxfId="52" priority="27" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="51" priority="28" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="41" priority="27" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="40" priority="28" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="top10" dxfId="50" priority="25" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="49" priority="26" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="39" priority="25" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="26" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="top10" dxfId="48" priority="23" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="47" priority="24" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="24" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="top10" dxfId="46" priority="21" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="45" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="top10" dxfId="44" priority="19" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="43" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="19" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="top10" dxfId="42" priority="17" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="41" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="17" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="top10" dxfId="40" priority="15" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="39" priority="16" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="15" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="16" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L11">
-    <cfRule type="top10" dxfId="38" priority="13" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="37" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="13" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="top10" dxfId="16" priority="12" percent="1" rank="10"/>
-    <cfRule type="top10" dxfId="17" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="top10" dxfId="14" priority="9" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="15" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="9" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M11">
-    <cfRule type="top10" dxfId="10" priority="7" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="11" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="7" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N11">
-    <cfRule type="top10" dxfId="9" priority="5" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="8" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O11">
-    <cfRule type="top10" dxfId="4" priority="3" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="5" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="3" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P11">
-    <cfRule type="top10" dxfId="3" priority="1" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="1" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>